<commit_message>
added initial test results of prefalign_prepilot
</commit_message>
<xml_diff>
--- a/XPlanningEvaluation/data/study/prefalign/prefalign_prepilot.xlsx
+++ b/XPlanningEvaluation/data/study/prefalign/prefalign_prepilot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rsukkerd/Projects/explainable-planning/XPlanningEvaluation/data/study/prefalign/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E10A76-7C1F-1F4B-997E-DA93D52B7C73}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F71441-3E9F-3040-B20D-CAD39CC11FF5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9620" yWindow="1300" windowWidth="27640" windowHeight="16940" xr2:uid="{67F88DD1-BBE0-8D41-AE9E-86AE49DB42B7}"/>
+    <workbookView xWindow="10760" yWindow="1440" windowWidth="27640" windowHeight="16940" xr2:uid="{67F88DD1-BBE0-8D41-AE9E-86AE49DB42B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Participant 1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Question ID</t>
   </si>
@@ -54,10 +54,40 @@
     <t>Confidence</t>
   </si>
   <si>
-    <t>Time</t>
-  </si>
-  <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>mission0</t>
+  </si>
+  <si>
+    <t>agentPolicy0</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Time (minutes)</t>
+  </si>
+  <si>
+    <t>mission13</t>
+  </si>
+  <si>
+    <t>agentPolicy1</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>mission26</t>
+  </si>
+  <si>
+    <t>agentPolicy2</t>
+  </si>
+  <si>
+    <t>Confident that optimality score of answer is &gt;= 0.95</t>
+  </si>
+  <si>
+    <t>Confident that optimality score of answer is &gt;=0.95</t>
   </si>
 </sst>
 </file>
@@ -409,17 +439,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3123FE25-4E55-FE47-B30B-9268259E5598}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -436,7 +468,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
         <v>6</v>
@@ -448,7 +480,73 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
         <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>3.48</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>3.26</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>4.33</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test results of PrefAlign prepilot with explanation
</commit_message>
<xml_diff>
--- a/XPlanningEvaluation/data/study/prefalign/prefalign_prepilot.xlsx
+++ b/XPlanningEvaluation/data/study/prefalign/prefalign_prepilot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rsukkerd/Projects/explainable-planning/XPlanningEvaluation/data/study/prefalign/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F71441-3E9F-3040-B20D-CAD39CC11FF5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59F43B3-C04B-974C-A4DE-88CAFDFCD4B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10760" yWindow="1440" windowWidth="27640" windowHeight="16940" xr2:uid="{67F88DD1-BBE0-8D41-AE9E-86AE49DB42B7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27600" windowHeight="19560" xr2:uid="{67F88DD1-BBE0-8D41-AE9E-86AE49DB42B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Participant 1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
   <si>
     <t>Question ID</t>
   </si>
@@ -88,6 +88,45 @@
   </si>
   <si>
     <t>Confident that optimality score of answer is &gt;=0.95</t>
+  </si>
+  <si>
+    <t>mission10</t>
+  </si>
+  <si>
+    <t>Confidence w/ Explanation</t>
+  </si>
+  <si>
+    <t>Time w/ Explanation</t>
+  </si>
+  <si>
+    <t>Answer w/ Explanation</t>
+  </si>
+  <si>
+    <t>mission20</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>mission30</t>
+  </si>
+  <si>
+    <t>Explanation didn't change mind; just confirmed.</t>
+  </si>
+  <si>
+    <t>mission40</t>
+  </si>
+  <si>
+    <t>agentPolicy3</t>
+  </si>
+  <si>
+    <t>Quick to answer: intrusive penalty is very high especially compared to time cost. Explanation didn't change mind; just confirmed.</t>
+  </si>
+  <si>
+    <t>Think another policy is a better but unsure; think they are close. Explanation improved confidence.</t>
+  </si>
+  <si>
+    <t>Think agentPolicy0 is good, but maybe there is another better policy. Wonder what happens if robot goes faster from L1-L2. Explanation changed mind.</t>
   </si>
 </sst>
 </file>
@@ -439,22 +478,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3123FE25-4E55-FE47-B30B-9268259E5598}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="44.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,22 +510,31 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>8</v>
       </c>
@@ -493,20 +544,32 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2">
         <v>3.48</v>
       </c>
-      <c r="F2">
-        <v>5</v>
-      </c>
       <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -516,17 +579,29 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3">
         <v>3.26</v>
       </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>24</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -536,17 +611,163 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4">
         <v>4.33</v>
       </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>24</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
       </c>
       <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>3.15</v>
+      </c>
+      <c r="G6">
+        <v>3.06</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8">
+        <v>2.23</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="J8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9">
+        <v>2.04</v>
+      </c>
+      <c r="G9">
+        <v>3.48</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="J9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>